<commit_message>
to wszystko ma byc
</commit_message>
<xml_diff>
--- a/serwi.xlsx
+++ b/serwi.xlsx
@@ -13439,7 +13439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13476,25 +13476,237 @@
     </row>
     <row r="2">
       <c r="A2" s="26" t="n">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RMA2110181431</t>
+          <t>2012221611-01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>X570D4U-2L2T</t>
+          <t>SSDSC2KB480G701</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>E7S0XW015927</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>PHYS81960047480BGN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>PHYS744100Z4480BGN</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="26" t="n">
+        <v>195</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2012221611-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSDSC2KB480G701</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PHYS819300CW480BGN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>BTYS82110B73480BGN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="26" t="n">
+        <v>196</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2012221611-03</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSDSC2KB480G701</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PHYS819300DB480BGN</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>BTYS807101X8480BGN</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="26" t="n">
+        <v>197</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2012221611-04</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SSDSC2KB480G701</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PHYS819301UT480BGN</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>PHYS738002M6480BGN</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="26" t="n">
+        <v>198</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2012221611-05</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SSDSC2KB480G701</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PHYS819301UW480BGN</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>PHYS7375003K480BGN</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="26" t="n">
+        <v>199</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2012221611-06</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SSDSC2KB480G701</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PHYS819300CZ480BGN</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>BTYS82010L38480BGN</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="26" t="n">
+        <v>200</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2012221611-07</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SSDSC2KB480G701</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PHYS819600HB480BGN</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>PHYS738000HY480BGN</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="26" t="n">
+        <v>201</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2012221611-08</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SSDSC2KB480G701</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PHYS816104DB480BGN</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>PHYS7375009W480BGN</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="26" t="n">
+        <v>202</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2012221611-09</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SSDSC2KB480G701</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PHYS819300NA480BGN</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>PHYS738000HH480BGN</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>